<commit_message>
Updated FRA model - 2025-08-07 15:49
</commit_message>
<xml_diff>
--- a/VerveStacks_FRA/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_FRA/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FRA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DEBF10-45A5-47A2-A237-A75C72AA6F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8F49DB-37DF-4027-B113-38430A5FDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -930,10 +930,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S6d1226h10,S1aH4,S2aH2,S6c1118h14,S6c1118h15,S6c1118h17,S6d1226h17,S1b0130h12,S1b0130h13,S6d1226h14,S6d1226h18,S4aH5,S6c1118h09,S6c1118h18,S1b0130h10,S3aH5,S5aH3,S6c1118h11,S6aH5,S6c1118h16,S6d1226h11,S1b0130h09,S6c1118h07,S6c1118h12,S6c1118h13,S1aH2,S1b0130h07,S2aH3,S6c1118h10,S1b0130h11,S3aH4,S4aH3,S4aH4,S6c1118h08,S1b0130h08,S3aH2,S1b0130h14,S1b0130h16,S3aH3,S1aH3,S6d1226h13,S6d1226h16,S1aH5,S1b0130h15,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S4aH2,S1b0130h17,S1b0130h18,S5aH4,S6aH3,S6aH4,S6d1226h07,S6d1226h08,S6d1226h09,S6d1226h12,S6d1226h15</t>
-  </si>
-  <si>
-    <t>S2aH8,S6c1118h06,S6c1118h21,S6d1226h05,S6d1226h19,S6d1226h22,S4aH1,S6aH1,S6d1226h24,S1aH1,S2aH7,S6d1226h20,S1b0130h21,S6c1118h23,S6d1226h02,S1aH8,S1b0130h03,S1b0130h24,S5aH1,S6aH7,S6c1118h01,S6c1118h02,S6c1118h05,S4aH8,S6c1118h03,S6c1118h20,S6d1226h04,S1b0130h02,S1b0130h06,S2aH6,S3aH1,S1b0130h20,S6c1118h22,S6d1226h21,S1b0130h23,S3aH8,S4aH6,S6d1226h06,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH6,S1b0130h04,S1b0130h19,S6c1118h04,S6c1118h24,S1b0130h22,S2aH1,S3aH7,S5aH8,S6c1118h19,S6d1226h01,S1b0130h01,S1b0130h05,S6aH8,S6d1226h03,S6d1226h23</t>
+    <t>S1aH5,S1b0130h15,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6d1226h10,S1b0130h12,S1b0130h13,S6d1226h14,S6d1226h18,S4aH2,S4aH5,S6c1118h09,S6c1118h18,S1b0130h18,S5aH4,S6aH3,S6aH4,S6d1226h07,S6d1226h08,S6d1226h09,S6d1226h12,S6d1226h15,S1b0130h11,S3aH4,S4aH3,S4aH4,S6c1118h08,S1b0130h10,S3aH5,S5aH3,S6c1118h11,S1b0130h08,S3aH2,S1aH2,S1b0130h07,S2aH3,S6c1118h10,S1b0130h14,S1b0130h16,S3aH3,S6aH5,S6c1118h16,S6d1226h11,S1b0130h17,S1b0130h09,S6c1118h07,S6c1118h12,S6c1118h13,S1aH3,S6d1226h13,S6d1226h16,S1aH4,S2aH2,S6c1118h14,S6c1118h15,S6c1118h17,S6d1226h17</t>
+  </si>
+  <si>
+    <t>S1aH6,S1b0130h04,S1b0130h19,S6c1118h04,S6c1118h24,S2aH8,S6c1118h06,S6c1118h21,S6d1226h05,S6d1226h19,S6d1226h22,S1aH1,S2aH7,S6d1226h20,S1b0130h22,S2aH1,S3aH7,S5aH8,S6c1118h19,S6d1226h01,S1b0130h21,S6c1118h23,S6d1226h02,S6d1226h23,S6d1226h21,S1aH8,S1b0130h03,S1b0130h24,S5aH1,S6aH7,S6c1118h01,S6c1118h02,S6c1118h05,S1b0130h23,S3aH8,S1b0130h20,S6c1118h22,S4aH6,S6d1226h06,S4aH8,S6c1118h03,S6c1118h20,S6d1226h04,S1b0130h01,S1b0130h05,S6aH8,S6d1226h03,S1b0130h02,S1b0130h06,S2aH6,S3aH1,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S4aH1,S6aH1,S6d1226h24</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S2aH8,S6c1118h06,S6c1118h21,S6d1226h05,S6d1226h19,S6d1226h22,S4aH1,S6aH1,S6d1226h24,S1aH1,S2aH7,S6d1226h20,S1b0130h21,S6c1118h23,S6d1226h02,S1aH8,S1b0130h03,S1b0130h24,S5aH1,S6aH7,S6c1118h01,S6c1118h02,S6c1118h05,S4aH8,S6c1118h03,S6c1118h20,S6d1226h04,S1b0130h02,S1b0130h06,S2aH6,S3aH1,S1b0130h20,S6c1118h22,S6d1226h21,S1b0130h23,S3aH8,S4aH6,S6d1226h06,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH6,S1b0130h04,S1b0130h19,S6c1118h04,S6c1118h24,S1b0130h22,S2aH1,S3aH7,S5aH8,S6c1118h19,S6d1226h01,S1b0130h01,S1b0130h05,S6aH8,S6d1226h03,S6d1226h23</v>
+        <v>S1aH6,S1b0130h04,S1b0130h19,S6c1118h04,S6c1118h24,S2aH8,S6c1118h06,S6c1118h21,S6d1226h05,S6d1226h19,S6d1226h22,S1aH1,S2aH7,S6d1226h20,S1b0130h22,S2aH1,S3aH7,S5aH8,S6c1118h19,S6d1226h01,S1b0130h21,S6c1118h23,S6d1226h02,S6d1226h23,S6d1226h21,S1aH8,S1b0130h03,S1b0130h24,S5aH1,S6aH7,S6c1118h01,S6c1118h02,S6c1118h05,S1b0130h23,S3aH8,S1b0130h20,S6c1118h22,S4aH6,S6d1226h06,S4aH8,S6c1118h03,S6c1118h20,S6d1226h04,S1b0130h01,S1b0130h05,S6aH8,S6d1226h03,S1b0130h02,S1b0130h06,S2aH6,S3aH1,S1aH7,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S4aH1,S6aH1,S6d1226h24</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S6d1226h10,S1aH4,S2aH2,S6c1118h14,S6c1118h15,S6c1118h17,S6d1226h17,S1b0130h12,S1b0130h13,S6d1226h14,S6d1226h18,S4aH5,S6c1118h09,S6c1118h18,S1b0130h10,S3aH5,S5aH3,S6c1118h11,S6aH5,S6c1118h16,S6d1226h11,S1b0130h09,S6c1118h07,S6c1118h12,S6c1118h13,S1aH2,S1b0130h07,S2aH3,S6c1118h10,S1b0130h11,S3aH4,S4aH3,S4aH4,S6c1118h08,S1b0130h08,S3aH2,S1b0130h14,S1b0130h16,S3aH3,S1aH3,S6d1226h13,S6d1226h16,S1aH5,S1b0130h15,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S4aH2,S1b0130h17,S1b0130h18,S5aH4,S6aH3,S6aH4,S6d1226h07,S6d1226h08,S6d1226h09,S6d1226h12,S6d1226h15</v>
+        <v>S1aH5,S1b0130h15,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6d1226h10,S1b0130h12,S1b0130h13,S6d1226h14,S6d1226h18,S4aH2,S4aH5,S6c1118h09,S6c1118h18,S1b0130h18,S5aH4,S6aH3,S6aH4,S6d1226h07,S6d1226h08,S6d1226h09,S6d1226h12,S6d1226h15,S1b0130h11,S3aH4,S4aH3,S4aH4,S6c1118h08,S1b0130h10,S3aH5,S5aH3,S6c1118h11,S1b0130h08,S3aH2,S1aH2,S1b0130h07,S2aH3,S6c1118h10,S1b0130h14,S1b0130h16,S3aH3,S6aH5,S6c1118h16,S6d1226h11,S1b0130h17,S1b0130h09,S6c1118h07,S6c1118h12,S6c1118h13,S1aH3,S6d1226h13,S6d1226h16,S1aH4,S2aH2,S6c1118h14,S6c1118h15,S6c1118h17,S6d1226h17</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2149,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E32086-EEC5-44D3-9937-26ADDB4D7C38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B87E67-B4AF-4D8D-A5D2-CF8A40940F08}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2866,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D759D3-66F4-4EE6-BDF1-B69D1A03D3EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D767DDF-0517-4D47-B49F-42E08CF5C6C1}">
   <dimension ref="B2:O123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2948,7 +2948,7 @@
         <v>85</v>
       </c>
       <c r="N4">
-        <v>6.2951773525791663E-2</v>
+        <v>6.2951773525791649E-2</v>
       </c>
       <c r="O4" t="s">
         <v>303</v>
@@ -2980,10 +2980,10 @@
         <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N5">
-        <v>0.24146805415687594</v>
+        <v>0.52122636231397557</v>
       </c>
       <c r="O5" t="s">
         <v>303</v>
@@ -3015,10 +3015,10 @@
         <v>171</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N6">
-        <v>0.52122636231397568</v>
+        <v>0.12315094550744095</v>
       </c>
       <c r="O6" t="s">
         <v>303</v>
@@ -3050,10 +3050,10 @@
         <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="N7">
-        <v>7.2664204990488979E-2</v>
+        <v>0.24146805415687592</v>
       </c>
       <c r="O7" t="s">
         <v>303</v>
@@ -3085,10 +3085,10 @@
         <v>171</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="N8">
-        <v>0.12315094550744098</v>
+        <v>0.17853865950542688</v>
       </c>
       <c r="O8" t="s">
         <v>303</v>
@@ -3120,10 +3120,10 @@
         <v>171</v>
       </c>
       <c r="M9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N9">
-        <v>0.17853865950542691</v>
+        <v>7.2664204990488979E-2</v>
       </c>
       <c r="O9" t="s">
         <v>303</v>
@@ -6099,7 +6099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB39A61D-7DAD-4C23-BFAD-F24E7CB35BF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C38BE48-E2B4-4B5E-800E-861AB853C3F8}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>